<commit_message>
Adjusted index.html for better mobile appearance
The buttons for "travel map" are now aligned in the same row.
</commit_message>
<xml_diff>
--- a/RouteAnalyses.xlsx
+++ b/RouteAnalyses.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent Wong\Documents\GitHub\alt-routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A3893F-5327-4174-94DA-C20C42491B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3982E4-E624-44A0-8D1F-688BCF3B77CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D895ED9F-9B08-45B6-A4C9-4605780550AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D895ED9F-9B08-45B6-A4C9-4605780550AB}"/>
   </bookViews>
   <sheets>
     <sheet name="CuhkToAdjacent" sheetId="1" r:id="rId1"/>
     <sheet name="CuhkToFar" sheetId="2" r:id="rId2"/>
+    <sheet name="TsingSha_X" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Plan Name</t>
   </si>
@@ -119,6 +120,27 @@
   </si>
   <si>
     <t>Shatin Central</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Fare</t>
+  </si>
+  <si>
+    <t>249X</t>
+  </si>
+  <si>
+    <t>280X</t>
+  </si>
+  <si>
+    <t>286X</t>
+  </si>
+  <si>
+    <t>287X</t>
+  </si>
+  <si>
+    <t>Rule: Take Max</t>
   </si>
 </sst>
 </file>
@@ -479,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFCD2FA-EF32-45D2-A9D5-273779771C9A}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -1744,4 +1766,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CC9B61-8D3A-49E2-9612-CDC571D97048}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>7.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>